<commit_message>
Add CSV Builder class
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proje\csv_builder\tera4energycsvbuilder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D87CC859-2BFD-41DB-8F26-F7E85649C661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C38F59BB-C3C0-498D-AFD4-272DA3D4ACE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14355" yWindow="1245" windowWidth="41970" windowHeight="13305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1995" yWindow="1260" windowWidth="22455" windowHeight="13305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plant" sheetId="1" r:id="rId1"/>
@@ -26,67 +26,109 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
-  <si>
-    <t>mohsen1</t>
-  </si>
-  <si>
-    <t>mohsen2</t>
-  </si>
-  <si>
-    <t>mohsen3</t>
-  </si>
-  <si>
-    <t>aa</t>
-  </si>
-  <si>
-    <t>bb</t>
-  </si>
-  <si>
-    <t>cc</t>
-  </si>
-  <si>
-    <t>dd</t>
-  </si>
-  <si>
-    <t>ee</t>
-  </si>
-  <si>
-    <t>ff</t>
-  </si>
-  <si>
-    <t>gg</t>
-  </si>
-  <si>
-    <t>ivan1</t>
-  </si>
-  <si>
-    <t>ivan2</t>
-  </si>
-  <si>
-    <t>ivan3</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
   <si>
     <t>Hostname Edge</t>
   </si>
   <si>
-    <t>beetasomething1</t>
-  </si>
-  <si>
-    <t>beetasomething2</t>
-  </si>
-  <si>
-    <t>beetasomething3</t>
-  </si>
-  <si>
-    <t>gioe</t>
+    <t>Edificio</t>
+  </si>
+  <si>
+    <t>Reparto</t>
+  </si>
+  <si>
+    <t>Linea</t>
+  </si>
+  <si>
+    <t>ID Modbus</t>
+  </si>
+  <si>
+    <t>beetamocob68a3b</t>
+  </si>
+  <si>
+    <t>beetamocob689fb</t>
+  </si>
+  <si>
+    <t>beetamocob37376</t>
+  </si>
+  <si>
+    <t>GioE-187E63</t>
+  </si>
+  <si>
+    <t>PC1</t>
+  </si>
+  <si>
+    <t>PC2</t>
+  </si>
+  <si>
+    <t>PC3</t>
+  </si>
+  <si>
+    <t>PC4</t>
+  </si>
+  <si>
+    <t>TERA1</t>
+  </si>
+  <si>
+    <t>TERA2</t>
+  </si>
+  <si>
+    <t>TERA3</t>
+  </si>
+  <si>
+    <t>TERA4</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>GC1</t>
+  </si>
+  <si>
+    <t>GC2</t>
+  </si>
+  <si>
+    <t>GC3</t>
+  </si>
+  <si>
+    <t>LC1</t>
+  </si>
+  <si>
+    <t>LC2</t>
+  </si>
+  <si>
+    <t>modbus-fc</t>
+  </si>
+  <si>
+    <t>modbus-address</t>
+  </si>
+  <si>
+    <t>Misura</t>
+  </si>
+  <si>
+    <t>Phase 1 Active Power</t>
+  </si>
+  <si>
+    <t>Phase 2 Active Power</t>
+  </si>
+  <si>
+    <t>Phase 3 Active Power</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,13 +136,43 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -115,8 +187,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,88 +473,207 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
+      <c r="E11">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -488,42 +683,46 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
+        <v>4140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
+        <v>4142</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -531,10 +730,10 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
+        <v>4144</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>